<commit_message>
second commit after adding more test cases
</commit_message>
<xml_diff>
--- a/com.sevenmartsupermarket/src/main/resources/testdata/testdataExcel.xlsx
+++ b/com.sevenmartsupermarket/src/main/resources/testdata/testdataExcel.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anakh\eclipse-workspace\com.sevenmartsupermarket\src\main\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anakh\git\SevenrmartSupermarket\com.sevenmartsupermarket\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3053CED-86EC-4F18-939C-405381CE342A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1216DC20-52FD-46DD-94E6-9DF95C091B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2832" yWindow="960" windowWidth="17280" windowHeight="8964" xr2:uid="{B3DD62FC-5046-4ADE-AD1A-523F18D8C2B6}"/>
+    <workbookView xWindow="2832" yWindow="960" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{B3DD62FC-5046-4ADE-AD1A-523F18D8C2B6}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminUserTestdata" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Username</t>
   </si>
@@ -40,6 +41,15 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>admin1</t>
   </si>
 </sst>
 </file>
@@ -393,7 +403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6CE0030-5D55-4B07-91BE-B3037AAD34E1}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -437,4 +447,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E02E3C4-3446-472A-B3A9-D60C9D3A232D}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>